<commit_message>
mullartiger Moder zu F-Mull geändert
</commit_message>
<xml_diff>
--- a/tabelle1.xlsx
+++ b/tabelle1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="984" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="983" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="tabelle" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="224">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -305,9 +305,6 @@
   </si>
   <si>
     <t xml:space="preserve">4.1a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mullartiger Moder</t>
   </si>
   <si>
     <t xml:space="preserve">38</t>
@@ -810,26 +807,25 @@
   <dimension ref="A1:P61"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P17" activeCellId="0" sqref="P17"/>
+      <selection pane="topLeft" activeCell="H28" activeCellId="0" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.63775510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.86734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.68877551020408"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="2.38265306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.24489795918367"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.45408163265306"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="4.43877551020408"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.484693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="5.3469387755102"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.2755102040816"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.9132653061224"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.8520408163265"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.82142857142857"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.89285714285714"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="51.0459183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="12.2755102040816"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.58673469387755"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.79591836734694"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="4.66326530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.5051020408163"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="5.68877551020408"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.09183673469388"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.9387755102041"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.75"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.16326530612245"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.5765306122449"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="54.5612244897959"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2033,7 +2029,7 @@
         <v>43</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>95</v>
+        <v>19</v>
       </c>
       <c r="I26" s="0" t="n">
         <v>7.33</v>
@@ -2059,10 +2055,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" s="0" t="s">
         <v>96</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>97</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>4</v>
@@ -2077,10 +2073,10 @@
         <v>39</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>95</v>
+        <v>19</v>
       </c>
       <c r="I27" s="0" t="n">
         <v>7.29</v>
@@ -2106,10 +2102,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B28" s="0" t="s">
         <v>99</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>100</v>
       </c>
       <c r="C28" s="0" t="n">
         <v>4</v>
@@ -2124,7 +2120,7 @@
         <v>261</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H28" s="0" t="s">
         <v>19</v>
@@ -2153,10 +2149,10 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" s="0" t="s">
         <v>102</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>103</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>4</v>
@@ -2171,13 +2167,13 @@
         <v>148</v>
       </c>
       <c r="G29" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="I29" s="0" t="s">
         <v>104</v>
-      </c>
-      <c r="H29" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="I29" s="0" t="s">
-        <v>105</v>
       </c>
       <c r="J29" s="0" t="n">
         <v>0</v>
@@ -2198,15 +2194,15 @@
         <v>0</v>
       </c>
       <c r="P29" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B30" s="0" t="s">
         <v>107</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>108</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>4</v>
@@ -2221,13 +2217,13 @@
         <v>296</v>
       </c>
       <c r="G30" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="I30" s="0" t="s">
         <v>109</v>
-      </c>
-      <c r="H30" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="I30" s="0" t="s">
-        <v>110</v>
       </c>
       <c r="J30" s="0" t="n">
         <v>0</v>
@@ -2248,15 +2244,15 @@
         <v>0</v>
       </c>
       <c r="P30" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B31" s="0" t="s">
         <v>112</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>113</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>4</v>
@@ -2271,13 +2267,13 @@
         <v>233</v>
       </c>
       <c r="G31" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="H31" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="I31" s="0" t="s">
         <v>114</v>
-      </c>
-      <c r="H31" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="I31" s="0" t="s">
-        <v>115</v>
       </c>
       <c r="J31" s="0" t="n">
         <v>0</v>
@@ -2300,10 +2296,10 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B32" s="0" t="s">
         <v>116</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>117</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>4</v>
@@ -2318,13 +2314,13 @@
         <v>282</v>
       </c>
       <c r="G32" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="H32" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="I32" s="0" t="s">
         <v>118</v>
-      </c>
-      <c r="H32" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="I32" s="0" t="s">
-        <v>119</v>
       </c>
       <c r="J32" s="0" t="n">
         <v>0</v>
@@ -2345,15 +2341,15 @@
         <v>0</v>
       </c>
       <c r="P32" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B33" s="0" t="s">
         <v>121</v>
-      </c>
-      <c r="B33" s="0" t="s">
-        <v>122</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>4</v>
@@ -2368,13 +2364,13 @@
         <v>199</v>
       </c>
       <c r="G33" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="H33" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="I33" s="0" t="s">
         <v>123</v>
-      </c>
-      <c r="H33" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="I33" s="0" t="s">
-        <v>124</v>
       </c>
       <c r="J33" s="0" t="n">
         <v>0</v>
@@ -2395,15 +2391,15 @@
         <v>0</v>
       </c>
       <c r="P33" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B34" s="0" t="s">
         <v>126</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>127</v>
       </c>
       <c r="C34" s="0" t="n">
         <v>4</v>
@@ -2418,13 +2414,13 @@
         <v>191</v>
       </c>
       <c r="G34" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="I34" s="0" t="s">
         <v>128</v>
-      </c>
-      <c r="H34" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="I34" s="0" t="s">
-        <v>129</v>
       </c>
       <c r="J34" s="0" t="n">
         <v>0</v>
@@ -2447,10 +2443,10 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B35" s="0" t="s">
         <v>130</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>131</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>4</v>
@@ -2465,13 +2461,13 @@
         <v>284</v>
       </c>
       <c r="G35" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="H35" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="I35" s="0" t="s">
         <v>132</v>
-      </c>
-      <c r="H35" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="I35" s="0" t="s">
-        <v>133</v>
       </c>
       <c r="J35" s="0" t="n">
         <v>0</v>
@@ -2494,10 +2490,10 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B36" s="0" t="s">
         <v>134</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>135</v>
       </c>
       <c r="C36" s="0" t="n">
         <v>4</v>
@@ -2512,13 +2508,13 @@
         <v>8</v>
       </c>
       <c r="G36" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="H36" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="I36" s="0" t="s">
         <v>136</v>
-      </c>
-      <c r="H36" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="I36" s="0" t="s">
-        <v>137</v>
       </c>
       <c r="J36" s="0" t="n">
         <v>0</v>
@@ -2541,10 +2537,10 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B37" s="0" t="s">
         <v>138</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>139</v>
       </c>
       <c r="C37" s="0" t="n">
         <v>4</v>
@@ -2559,13 +2555,13 @@
         <v>172</v>
       </c>
       <c r="G37" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="I37" s="0" t="s">
         <v>140</v>
-      </c>
-      <c r="H37" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="I37" s="0" t="s">
-        <v>141</v>
       </c>
       <c r="J37" s="0" t="n">
         <v>0</v>
@@ -2588,10 +2584,10 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B38" s="0" t="s">
         <v>142</v>
-      </c>
-      <c r="B38" s="0" t="s">
-        <v>143</v>
       </c>
       <c r="C38" s="0" t="n">
         <v>5</v>
@@ -2606,13 +2602,13 @@
         <v>187</v>
       </c>
       <c r="G38" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="H38" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="I38" s="0" t="s">
         <v>144</v>
-      </c>
-      <c r="H38" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="I38" s="0" t="s">
-        <v>145</v>
       </c>
       <c r="J38" s="0" t="n">
         <v>0</v>
@@ -2635,10 +2631,10 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B39" s="0" t="s">
         <v>146</v>
-      </c>
-      <c r="B39" s="0" t="s">
-        <v>147</v>
       </c>
       <c r="C39" s="0" t="n">
         <v>5</v>
@@ -2653,13 +2649,13 @@
         <v>249</v>
       </c>
       <c r="G39" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="H39" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="I39" s="0" t="s">
         <v>148</v>
-      </c>
-      <c r="H39" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="I39" s="0" t="s">
-        <v>149</v>
       </c>
       <c r="J39" s="0" t="n">
         <v>0</v>
@@ -2682,10 +2678,10 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B40" s="0" t="s">
         <v>150</v>
-      </c>
-      <c r="B40" s="0" t="s">
-        <v>151</v>
       </c>
       <c r="C40" s="0" t="n">
         <v>5</v>
@@ -2700,13 +2696,13 @@
         <v>172</v>
       </c>
       <c r="G40" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="H40" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="I40" s="0" t="s">
         <v>152</v>
-      </c>
-      <c r="H40" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="I40" s="0" t="s">
-        <v>153</v>
       </c>
       <c r="J40" s="0" t="n">
         <v>0</v>
@@ -2729,10 +2725,10 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B41" s="0" t="s">
         <v>154</v>
-      </c>
-      <c r="B41" s="0" t="s">
-        <v>155</v>
       </c>
       <c r="C41" s="0" t="n">
         <v>5</v>
@@ -2753,7 +2749,7 @@
         <v>40</v>
       </c>
       <c r="I41" s="0" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J41" s="0" t="n">
         <v>0</v>
@@ -2776,10 +2772,10 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B42" s="0" t="s">
         <v>157</v>
-      </c>
-      <c r="B42" s="0" t="s">
-        <v>158</v>
       </c>
       <c r="C42" s="0" t="n">
         <v>5</v>
@@ -2794,13 +2790,13 @@
         <v>158</v>
       </c>
       <c r="G42" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="H42" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="I42" s="0" t="s">
         <v>159</v>
-      </c>
-      <c r="H42" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="I42" s="0" t="s">
-        <v>160</v>
       </c>
       <c r="J42" s="0" t="n">
         <v>0</v>
@@ -2823,10 +2819,10 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B43" s="0" t="s">
         <v>161</v>
-      </c>
-      <c r="B43" s="0" t="s">
-        <v>162</v>
       </c>
       <c r="C43" s="0" t="n">
         <v>5</v>
@@ -2841,13 +2837,13 @@
         <v>88</v>
       </c>
       <c r="G43" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="H43" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="I43" s="0" t="s">
         <v>163</v>
-      </c>
-      <c r="H43" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="I43" s="0" t="s">
-        <v>164</v>
       </c>
       <c r="J43" s="0" t="n">
         <v>0</v>
@@ -2870,10 +2866,10 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B44" s="0" t="s">
         <v>165</v>
-      </c>
-      <c r="B44" s="0" t="s">
-        <v>166</v>
       </c>
       <c r="C44" s="0" t="n">
         <v>5</v>
@@ -2888,13 +2884,13 @@
         <v>25</v>
       </c>
       <c r="G44" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="H44" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="I44" s="0" t="s">
         <v>167</v>
-      </c>
-      <c r="H44" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="I44" s="0" t="s">
-        <v>168</v>
       </c>
       <c r="J44" s="0" t="n">
         <v>0</v>
@@ -2917,10 +2913,10 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B45" s="0" t="s">
         <v>169</v>
-      </c>
-      <c r="B45" s="0" t="s">
-        <v>170</v>
       </c>
       <c r="C45" s="0" t="n">
         <v>5</v>
@@ -2935,13 +2931,13 @@
         <v>36</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H45" s="0" t="s">
         <v>40</v>
       </c>
       <c r="I45" s="0" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J45" s="0" t="n">
         <v>0</v>
@@ -2964,10 +2960,10 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B46" s="0" t="s">
         <v>172</v>
-      </c>
-      <c r="B46" s="0" t="s">
-        <v>173</v>
       </c>
       <c r="C46" s="0" t="n">
         <v>5</v>
@@ -2982,13 +2978,13 @@
         <v>114</v>
       </c>
       <c r="G46" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="H46" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="I46" s="0" t="s">
         <v>174</v>
-      </c>
-      <c r="H46" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="I46" s="0" t="s">
-        <v>175</v>
       </c>
       <c r="J46" s="0" t="n">
         <v>0</v>
@@ -3011,10 +3007,10 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B47" s="0" t="s">
         <v>176</v>
-      </c>
-      <c r="B47" s="0" t="s">
-        <v>177</v>
       </c>
       <c r="C47" s="0" t="n">
         <v>5</v>
@@ -3029,13 +3025,13 @@
         <v>264</v>
       </c>
       <c r="G47" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="H47" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="I47" s="0" t="s">
         <v>178</v>
-      </c>
-      <c r="H47" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="I47" s="0" t="s">
-        <v>179</v>
       </c>
       <c r="J47" s="0" t="n">
         <v>0</v>
@@ -3058,10 +3054,10 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B48" s="0" t="s">
         <v>180</v>
-      </c>
-      <c r="B48" s="0" t="s">
-        <v>181</v>
       </c>
       <c r="C48" s="0" t="n">
         <v>5</v>
@@ -3076,7 +3072,7 @@
         <v>238</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H48" s="0" t="s">
         <v>19</v>
@@ -3105,10 +3101,10 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B49" s="0" t="s">
         <v>183</v>
-      </c>
-      <c r="B49" s="0" t="s">
-        <v>184</v>
       </c>
       <c r="C49" s="0" t="n">
         <v>5</v>
@@ -3123,13 +3119,13 @@
         <v>146</v>
       </c>
       <c r="G49" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="H49" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="I49" s="0" t="s">
         <v>185</v>
-      </c>
-      <c r="H49" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="I49" s="0" t="s">
-        <v>186</v>
       </c>
       <c r="J49" s="0" t="n">
         <v>0</v>
@@ -3152,10 +3148,10 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B50" s="0" t="s">
         <v>187</v>
-      </c>
-      <c r="B50" s="0" t="s">
-        <v>188</v>
       </c>
       <c r="C50" s="0" t="n">
         <v>6</v>
@@ -3170,13 +3166,13 @@
         <v>329</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H50" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I50" s="0" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J50" s="0" t="n">
         <v>0</v>
@@ -3199,10 +3195,10 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B51" s="0" t="s">
         <v>191</v>
-      </c>
-      <c r="B51" s="0" t="s">
-        <v>192</v>
       </c>
       <c r="C51" s="0" t="n">
         <v>6</v>
@@ -3217,13 +3213,13 @@
         <v>106</v>
       </c>
       <c r="G51" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="H51" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="I51" s="0" t="s">
         <v>193</v>
-      </c>
-      <c r="H51" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="I51" s="0" t="s">
-        <v>194</v>
       </c>
       <c r="J51" s="0" t="n">
         <v>0</v>
@@ -3246,10 +3242,10 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B52" s="0" t="s">
         <v>195</v>
-      </c>
-      <c r="B52" s="0" t="s">
-        <v>196</v>
       </c>
       <c r="C52" s="0" t="n">
         <v>6</v>
@@ -3264,13 +3260,13 @@
         <v>165</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H52" s="0" t="s">
         <v>40</v>
       </c>
       <c r="I52" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J52" s="0" t="n">
         <v>0</v>
@@ -3293,10 +3289,10 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B53" s="0" t="s">
         <v>198</v>
-      </c>
-      <c r="B53" s="0" t="s">
-        <v>199</v>
       </c>
       <c r="C53" s="0" t="n">
         <v>6</v>
@@ -3311,13 +3307,13 @@
         <v>120</v>
       </c>
       <c r="G53" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="H53" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="I53" s="0" t="s">
         <v>200</v>
-      </c>
-      <c r="H53" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="I53" s="0" t="s">
-        <v>201</v>
       </c>
       <c r="J53" s="0" t="n">
         <v>0</v>
@@ -3340,10 +3336,10 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B54" s="0" t="s">
         <v>202</v>
-      </c>
-      <c r="B54" s="0" t="s">
-        <v>203</v>
       </c>
       <c r="C54" s="0" t="n">
         <v>6</v>
@@ -3364,7 +3360,7 @@
         <v>40</v>
       </c>
       <c r="I54" s="0" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J54" s="0" t="n">
         <v>0</v>
@@ -3387,10 +3383,10 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B55" s="0" t="s">
         <v>205</v>
-      </c>
-      <c r="B55" s="0" t="s">
-        <v>206</v>
       </c>
       <c r="C55" s="0" t="n">
         <v>6</v>
@@ -3405,13 +3401,13 @@
         <v>93</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H55" s="0" t="s">
         <v>40</v>
       </c>
       <c r="I55" s="0" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J55" s="0" t="n">
         <v>0</v>
@@ -3434,10 +3430,10 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B56" s="0" t="s">
         <v>208</v>
-      </c>
-      <c r="B56" s="0" t="s">
-        <v>209</v>
       </c>
       <c r="C56" s="0" t="n">
         <v>6</v>
@@ -3452,7 +3448,7 @@
         <v>172</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H56" s="0" t="s">
         <v>40</v>
@@ -3481,10 +3477,10 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B57" s="0" t="s">
         <v>211</v>
-      </c>
-      <c r="B57" s="0" t="s">
-        <v>212</v>
       </c>
       <c r="C57" s="0" t="n">
         <v>6</v>
@@ -3499,7 +3495,7 @@
         <v>276</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H57" s="0" t="s">
         <v>40</v>
@@ -3528,10 +3524,10 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B58" s="0" t="s">
         <v>214</v>
-      </c>
-      <c r="B58" s="0" t="s">
-        <v>215</v>
       </c>
       <c r="C58" s="0" t="n">
         <v>6</v>
@@ -3546,7 +3542,7 @@
         <v>30</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H58" s="0" t="s">
         <v>40</v>
@@ -3575,10 +3571,10 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B59" s="0" t="s">
         <v>217</v>
-      </c>
-      <c r="B59" s="0" t="s">
-        <v>218</v>
       </c>
       <c r="C59" s="0" t="n">
         <v>6</v>
@@ -3593,7 +3589,7 @@
         <v>315</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H59" s="0" t="s">
         <v>40</v>
@@ -3622,10 +3618,10 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B60" s="0" t="s">
         <v>219</v>
-      </c>
-      <c r="B60" s="0" t="s">
-        <v>220</v>
       </c>
       <c r="C60" s="0" t="n">
         <v>6</v>
@@ -3640,7 +3636,7 @@
         <v>122</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H60" s="0" t="s">
         <v>40</v>
@@ -3669,10 +3665,10 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B61" s="0" t="s">
         <v>222</v>
-      </c>
-      <c r="B61" s="0" t="s">
-        <v>223</v>
       </c>
       <c r="C61" s="0" t="n">
         <v>6</v>
@@ -3687,7 +3683,7 @@
         <v>302</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H61" s="0" t="s">
         <v>40</v>

</xml_diff>